<commit_message>
Added details for modules, pcb, and housing.
</commit_message>
<xml_diff>
--- a/Project Details/BOM.xlsx
+++ b/Project Details/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="104">
   <si>
     <t>ITEM</t>
   </si>
@@ -280,6 +280,54 @@
   </si>
   <si>
     <t>NO-SHOULD BE OK</t>
+  </si>
+  <si>
+    <t>JMP1</t>
+  </si>
+  <si>
+    <t>SHUNT/JUMPER</t>
+  </si>
+  <si>
+    <t>4-881545-2</t>
+  </si>
+  <si>
+    <t>A26853-ND</t>
+  </si>
+  <si>
+    <t>RF Module 10 Pack</t>
+  </si>
+  <si>
+    <t>NRF24L01+</t>
+  </si>
+  <si>
+    <t>EBAY</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>IR 1</t>
+  </si>
+  <si>
+    <t>RF 1</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>IR SENSOR</t>
+  </si>
+  <si>
+    <t>PCB BOARDS</t>
+  </si>
+  <si>
+    <t>HS1</t>
+  </si>
+  <si>
+    <t>HOUSING</t>
   </si>
 </sst>
 </file>
@@ -392,7 +440,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -442,6 +490,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -747,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,7 +875,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="H2" s="5">
-        <f t="shared" ref="H2:H21" si="0" xml:space="preserve"> G2 * F2</f>
+        <f t="shared" ref="H2:H22" si="0" xml:space="preserve"> G2 * F2</f>
         <v>1.44</v>
       </c>
       <c r="I2" s="9" t="s">
@@ -1401,54 +1454,143 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F21" s="4">
-        <v>10</v>
-      </c>
-      <c r="G21" s="4">
-        <v>0.41099999999999998</v>
-      </c>
-      <c r="H21" s="25">
-        <f t="shared" si="0"/>
-        <v>4.1099999999999994</v>
-      </c>
-      <c r="I21" s="4" t="s">
+      <c r="A21" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="6">
+        <v>25</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="H21" s="5">
+        <f t="shared" si="0"/>
+        <v>6.4249999999999998</v>
+      </c>
+      <c r="I21" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="J21" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22" s="4">
+        <v>10</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="H22" s="25">
+        <f t="shared" si="0"/>
+        <v>4.1099999999999994</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="2">
-        <f>SUM(H2:H21)</f>
-        <v>97.990000000000009</v>
-      </c>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="2">
+        <f>SUM(H2:H22)</f>
+        <v>104.41500000000001</v>
+      </c>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>17.28</v>
+      </c>
+      <c r="I26" t="s">
+        <v>95</v>
+      </c>
+      <c r="J26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" t="s">
+        <v>100</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" t="s">
+        <v>101</v>
+      </c>
+      <c r="F28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" t="s">
+        <v>103</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>